<commit_message>
removed check that tower nodes need to start at 0 (tower mesh should start at TwrBsHt) added some insurance that TowerLoad%nnodes gets initialized to 0 when TwrAero isn't used
git-svn-id: https://windsvn2.nrel.gov/WT_Perf/branches/v4.x@135 a6739609-9c9d-4a29-a9ec-bdd8708b3f03

Former-commit-id: 3ea93155338ad1a7ad09c567dcb17723873b2ad3
</commit_message>
<xml_diff>
--- a/modules-local/aerodyn/src/OutListParameters.xlsx
+++ b/modules-local/aerodyn/src/OutListParameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="300" windowWidth="15240" windowHeight="7848" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="300" windowWidth="11928" windowHeight="5424" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -7162,8 +7162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1080"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1049" workbookViewId="0">
-      <selection activeCell="F1078" sqref="F1078:F1080"/>
+    <sheetView tabSelected="1" topLeftCell="A1048" workbookViewId="0">
+      <selection activeCell="B1066" sqref="B1066"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>